<commit_message>
added eda for cleaned data
</commit_message>
<xml_diff>
--- a/analysis/eda_cleaned_data.xlsx
+++ b/analysis/eda_cleaned_data.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>numrate</t>
+          <t>mths_since_last_delinq</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -465,16 +465,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>10000</v>
+        <v>5424</v>
       </c>
       <c r="D2" t="n">
-        <v>100</v>
+        <v>56.95086098278035</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>num_rate</t>
+          <t>emp_length</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -483,124 +483,124 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>10000</v>
+        <v>405</v>
       </c>
       <c r="D3" t="n">
-        <v>100</v>
+        <v>4.252414951700966</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>interest_rate</t>
+          <t>id</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>int64</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>wtd_loans</t>
+          <t>is_bad_loan</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>bool</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>mths_since_last_delinq</t>
+          <t>days_since_earliest_cr_line</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>int64</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5900</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>emp_length</t>
+          <t>total_rec_int</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>object</t>
+          <t>float64</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>881</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>8.81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>earliest_cr_line</t>
+          <t>total_rec_prncp</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>object</t>
+          <t>float64</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>4.760000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>int_rate2</t>
+          <t>total_pymnt</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>object</t>
+          <t>float64</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>4.760000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>total_rec_int</t>
+          <t>out_prncp</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -609,16 +609,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>4.760000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>total_rec_prncp</t>
+          <t>total_acc</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -627,16 +627,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>4.760000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>total_pymnt</t>
+          <t>revol_bal</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -645,16 +645,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>4.760000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>out_prncp</t>
+          <t>open_acc</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -663,16 +663,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>4.760000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>total_acc</t>
+          <t>delinq_2yrs</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -681,34 +681,34 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>4.760000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>revol_bal</t>
+          <t>loan_amnt</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>int64</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>4.760000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>open_acc</t>
+          <t>dti</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -717,52 +717,52 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>4.760000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>int_rate3</t>
+          <t>addr_state</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>object</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>4.760000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>delinq_2yrs</t>
+          <t>purpose</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>object</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>4.760000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>dti</t>
+          <t>annual_inc</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -771,16 +771,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>4.760000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>purpose</t>
+          <t>home_ownership</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -789,34 +789,34 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>4.760000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>loan_status</t>
+          <t>installment</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>object</t>
+          <t>float64</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>4.760000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>annual_inc</t>
+          <t>int_rate</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -825,153 +825,63 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>4.760000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>home_ownership</t>
+          <t>term</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>object</t>
+          <t>float64</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>4.760000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>installment</t>
+          <t>funded_amnt</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>int64</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>4.760000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>int_rate</t>
+          <t>is_loan_complete</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>bool</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>476</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>4.760000000000001</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>term</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>object</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>476</v>
-      </c>
-      <c r="D26" t="n">
-        <v>4.760000000000001</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>loan_amnt</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>int64</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>addr_state</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>object</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="inlineStr">
-        <is>
-          <t>funded_amnt</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>int64</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>int64</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -986,7 +896,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1049,39 +959,39 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>term</t>
+          <t>home_ownership</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[' 60 months' ' 36 months' nan]</t>
+          <t>['MORTGAGE' 'RENT' 'OWN' 'OTHER' 'NONE']</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[' 36 months', ' 60 months']</t>
+          <t>['MORTGAGE', 'RENT', 'OWN']</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[' 36 months', ' 60 months']</t>
+          <t>['MORTGAGE', 'RENT', 'OWN']</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[' 36 months', ' 60 months']</t>
+          <t>['MORTGAGE', 'RENT', 'OWN']</t>
         </is>
       </c>
       <c r="J2" t="n">
@@ -1089,212 +999,69 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>[' 36 months', ' 60 months']</t>
+          <t>['MORTGAGE', 'RENT']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>emp_length</t>
+          <t>purpose</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['10+ years' '2 years' '3 years' '7 years' '6 years' '4 years' '5 years'
- '8 years' nan '1 year' '&lt; 1 year' '9 years']</t>
+          <t>['credit_card' 'small_business' 'debt_consolidation' 'home_improvement'
+ 'other' 'wedding' 'major_purchase' 'car' 'house' 'renewable_energy'
+ 'vacation' 'medical' 'moving']</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['10+ years', '2 years', '5 years', '3 years', '&lt; 1 year', '6 years', '1 year', '7 years', '4 years', '8 years', '9 years']</t>
+          <t>['debt_consolidation', 'credit_card', 'home_improvement', 'other', 'major_purchase', 'small_business', 'car', 'medical', 'wedding', 'house', 'vacation', 'moving', 'renewable_energy']</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['10+ years', '2 years', '5 years', '3 years', '&lt; 1 year', '6 years', '1 year', '7 years', '4 years', '8 years', '9 years']</t>
+          <t>['debt_consolidation', 'credit_card', 'home_improvement', 'other', 'major_purchase', 'small_business']</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>['10+ years', '2 years', '5 years', '3 years', '&lt; 1 year', '6 years', '1 year', '7 years', '4 years']</t>
+          <t>['debt_consolidation', 'credit_card', 'home_improvement']</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>['10+ years']</t>
+          <t>['debt_consolidation', 'credit_card']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>home_ownership</t>
+          <t>addr_state</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C4" t="inlineStr">
-        <is>
-          <t>['MORTGAGE' 'RENT' 'OWN' 'OTHER' 'NONE' nan]</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>['MORTGAGE', 'RENT', 'OWN']</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>3</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>['MORTGAGE', 'RENT', 'OWN']</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>3</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>['MORTGAGE', 'RENT', 'OWN']</t>
-        </is>
-      </c>
-      <c r="J4" t="n">
-        <v>2</v>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>['MORTGAGE', 'RENT']</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>loan_status</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>7</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>['Current' 'Late (31-120 days)' 'Fully Paid' 'Charged Off'
- 'Late (16-30 days)' 'In Grace Period' 'Default' nan]</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>7</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>['Current', 'Fully Paid', 'Charged Off', 'Late (31-120 days)', 'In Grace Period', 'Late (16-30 days)', 'Default']</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>4</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>['Current', 'Fully Paid', 'Charged Off', 'Late (31-120 days)']</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>['Current', 'Fully Paid']</t>
-        </is>
-      </c>
-      <c r="J5" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>['Current']</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>purpose</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>13</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>['credit_card' 'small_business' 'debt_consolidation' 'home_improvement'
- 'other' 'wedding' 'major_purchase' 'car' 'house' 'renewable_energy'
- 'vacation' 'medical' 'moving' nan]</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>12</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>['debt_consolidation', 'credit_card', 'home_improvement', 'other', 'major_purchase', 'small_business', 'car', 'medical', 'wedding', 'house', 'vacation', 'moving', 'renewable_energy']</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>6</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>['debt_consolidation', 'credit_card', 'home_improvement', 'other', 'major_purchase', 'small_business']</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>3</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>['debt_consolidation', 'credit_card', 'home_improvement']</t>
-        </is>
-      </c>
-      <c r="J6" t="n">
-        <v>2</v>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>['debt_consolidation', 'credit_card']</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>addr_state</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>45</v>
-      </c>
-      <c r="C7" t="inlineStr">
         <is>
           <t>['MA' 'WA' 'NY' 'NJ' 'VA' 'NV' 'CA' 'FL' 'TX' 'NM' 'NC' 'OH' 'AZ' 'SC'
  'CO' 'DE' 'CT' 'IL' 'WI' 'PA' 'MD' 'GA' 'MN' 'MI' 'LA' 'RI' 'MO' 'KS'
@@ -1302,147 +1069,36 @@
  'VT' 'IN' 'TN']</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D4" t="n">
         <v>43</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>['CA', 'NY', 'TX', 'FL', 'NJ', 'PA', 'IL', 'VA', 'GA', 'NC', 'OH', 'AZ', 'WA', 'MI', 'MD', 'CO', 'MA', 'MN', 'NV', 'CT', 'MO', 'SC', 'OR', 'IN', 'AL', 'WI', 'TN', 'LA', 'KY', 'OK', 'KS', 'UT', 'AR', 'HI', 'WV', 'NM', 'RI', 'NH', 'DC', 'WY', 'MT', 'SD', 'DE', 'AK', 'VT']</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>['CA', 'NY', 'TX', 'FL', 'NJ', 'PA', 'IL', 'VA', 'GA', 'OH', 'NC', 'WA', 'AZ', 'MI', 'MD', 'CO', 'MA', 'MN', 'NV', 'CT', 'MO', 'SC', 'OR', 'WI', 'AL', 'IN', 'TN', 'LA', 'KY', 'OK', 'KS', 'UT', 'AR', 'HI', 'WV', 'NM', 'RI', 'NH', 'DC', 'WY', 'MT', 'SD', 'DE', 'AK', 'VT']</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
         <v>27</v>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>['CA', 'NY', 'TX', 'FL', 'NJ', 'PA', 'IL', 'VA', 'GA', 'NC', 'OH', 'AZ', 'WA', 'MI', 'MD', 'CO', 'MA', 'MN', 'NV', 'CT', 'MO', 'SC', 'OR', 'IN', 'AL', 'WI', 'TN', 'LA', 'KY']</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>['CA', 'NY', 'TX', 'FL', 'NJ', 'PA', 'IL', 'VA', 'GA', 'OH', 'NC', 'WA', 'AZ', 'MI', 'MD', 'CO', 'MA', 'MN', 'NV', 'CT', 'MO', 'SC', 'OR', 'WI', 'AL', 'IN', 'TN', 'LA', 'KY']</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
         <v>4</v>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>['CA', 'NY', 'TX', 'FL']</t>
         </is>
       </c>
-      <c r="J7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" t="inlineStr">
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>['CA']</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>earliest_cr_line</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>9397</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>['1995-12-27 02:06:00' '1994-04-07 12:00:00' '1993-07-16 08:41:00' ...
- '1997-11-10 12:00:00' '1990-11-08 12:00:00' '1980-11-19 12:00:00']</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>int_rate2</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>134</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>['10.16%' '8.90%' '7.90%' '13.67%' '15.80%' '15.96%' '7.51%' '13.49%'
- '17.27%' '22.74%' '11.71%' '12.42%' '6.03%' '14.27%' '16.29%' '18.64%'
- '19.42%' '10.65%' '12.69%' '18.49%' '6.62%' '9.99%' '11.14%' '15.27%'
- '14.65%' '9.91%' '19.91%' '20.30%' '18.25%' '13.99%' '20.89%' '18.55%'
- '12.12%' '19.03%' '17.58%' '21.28%' '19.99%' '10.74%' '17.99%' '21.48%'
- '14.09%' '9.76%' '16.77%' '13.11%' '7.62%' '15.31%' '20.99%' '19.22%'
- '23.33%' '15.81%' '19.05%' '20.50%' '21.00%' '22.45%' '14.33%' '21.97%'
- '22.78%' '23.13%' '24.20%' '23.26%' '17.77%' '20.49%' '18.75%' '23.63%'
- '21.98%' '23.76%' '22.47%' '23.83%' '19.72%' '22.95%' '23.28%' '24.89%'
- '21.49%' '24.83%' '9.71%' '15.22%' '24.70%' '14.47%' '24.50%' '13.68%'
- '20.80%' '11.99%' '10.64%' '12.35%' '15.88%' '12.85%' '20.31%' '16.99%'
- '18.85%' '11.55%' '24.08%' '10.99%' '21.15%' '17.56%' '21.70%' '13.05%'
- '21.60%' '16.78%' '22.70%' '22.20%' '19.52%' '12.99%' '25.28%' '24.99%'
- '25.80%' '17.10%' '23.50%' '25.89%' '25.83%' '15.10%' '8.60%' '15.61%'
- '16.20%' '23.10%' '13.53%' '9.67%' '17.76%' '23.40%' '14.98%' '26.06%'
- '22.40%' '25.57%' '14.30%' '20.20%' '23.70%' '6.97%' '9.25%' '19.20%'
- '16.24%' '17.57%' '13.98%' '25.99%' '22.90%' '19.97%' nan]</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>75</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>['12.12%', '13.11%', '8.90%', '14.33%', '7.90%', '11.14%', '15.31%', '16.29%', '7.62%', '10.16%', '14.09%', '6.03%', '17.27%', '15.80%', '6.62%', '10.99%', '17.77%', '11.99%', '13.67%', '18.49%', '15.61%', '10.64%', '12.99%', '12.35%', '11.55%', '18.75%', '19.05%', '9.71%', '15.10%', '19.72%', '15.22%', '14.30%', '19.52%', '16.20%', '15.88%', '13.68%', '16.78%', '21.00%', '17.10%', '18.25%', '17.56%', '18.55%', '9.67%', '17.76%', '9.99%', '21.98%', '13.05%', '14.98%', '18.85%', '14.65%', '20.20%', '13.99%', '14.47%', '19.20%', '20.31%', '21.49%', '12.85%', '20.49%', '23.28%', '22.47%', '13.53%', '24.08%', '10.74%', '19.22%', '9.76%', '22.95%', '17.57%', '21.60%', '22.40%', '23.40%', '21.70%', '13.98%', '9.25%', '16.24%', '21.15%', '23.10%', '23.63%', '21.48%', '24.50%', '8.60%', '20.80%', '23.70%', '22.20%', '20.50%', '15.81%', '16.99%', '11.71%', '23.83%', '17.99%', '19.97%', '22.70%', '23.76%', '24.89%', '12.69%', '6.97%', '19.99%', '23.50%', '12.42%', '7.51%', '9.91%', '22.90%', '13.49%', '24.99%', '21.97%', '14.27%', '24.70%']</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>32</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>['12.12%', '13.11%', '8.90%', '14.33%', '7.90%', '11.14%', '15.31%', '16.29%', '7.62%', '10.16%', '14.09%', '6.03%', '17.27%', '15.80%', '6.62%', '10.99%', '17.77%', '11.99%', '13.67%', '18.49%', '15.61%', '10.64%', '12.99%', '12.35%', '11.55%', '18.75%', '19.05%', '9.71%', '15.10%', '19.72%', '15.22%', '14.30%', '19.52%', '16.20%']</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>['12.12%']</t>
-        </is>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1549,37 +1205,37 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10000</v>
+        <v>9524</v>
       </c>
       <c r="C2" t="n">
-        <v>5143647.8516</v>
+        <v>4996389.764804704</v>
       </c>
       <c r="D2" t="n">
-        <v>2827943.823265978</v>
+        <v>2806971.303970144</v>
       </c>
       <c r="E2" t="n">
         <v>571203</v>
       </c>
       <c r="F2" t="n">
-        <v>2300882.5</v>
+        <v>2091955</v>
       </c>
       <c r="G2" t="n">
-        <v>5605038.5</v>
+        <v>5155782</v>
       </c>
       <c r="H2" t="n">
-        <v>7435741</v>
+        <v>7266550.5</v>
       </c>
       <c r="I2" t="n">
         <v>10125066</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0344612332589416</v>
+        <v>0.1114134475865919</v>
       </c>
       <c r="K2" t="n">
-        <v>1099655.12</v>
+        <v>1098808.59</v>
       </c>
       <c r="L2" t="n">
-        <v>10100140.5</v>
+        <v>10099163.59</v>
       </c>
       <c r="M2" t="n">
         <v>1</v>
@@ -1591,7 +1247,7 @@
         <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>10000</v>
+        <v>9524</v>
       </c>
     </row>
     <row r="3">
@@ -1601,13 +1257,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10000</v>
+        <v>9524</v>
       </c>
       <c r="C3" t="n">
-        <v>14054.8075</v>
+        <v>14321.86843763125</v>
       </c>
       <c r="D3" t="n">
-        <v>8108.658727562763</v>
+        <v>8163.592826985727</v>
       </c>
       <c r="E3" t="n">
         <v>1000</v>
@@ -1616,19 +1272,19 @@
         <v>8000</v>
       </c>
       <c r="G3" t="n">
-        <v>12000</v>
+        <v>12112.5</v>
       </c>
       <c r="H3" t="n">
-        <v>19400</v>
+        <v>20000</v>
       </c>
       <c r="I3" t="n">
         <v>35000</v>
       </c>
       <c r="J3" t="n">
-        <v>0.7516776905398361</v>
+        <v>0.7150678969033651</v>
       </c>
       <c r="K3" t="n">
-        <v>1600</v>
+        <v>1680.75</v>
       </c>
       <c r="L3" t="n">
         <v>35000</v>
@@ -1643,7 +1299,7 @@
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="4">
@@ -1653,13 +1309,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10000</v>
+        <v>9524</v>
       </c>
       <c r="C4" t="n">
-        <v>14052.73</v>
+        <v>14319.68710625788</v>
       </c>
       <c r="D4" t="n">
-        <v>8107.693230262946</v>
+        <v>8162.657251032556</v>
       </c>
       <c r="E4" t="n">
         <v>1000</v>
@@ -1668,19 +1324,19 @@
         <v>8000</v>
       </c>
       <c r="G4" t="n">
-        <v>12000</v>
+        <v>12112.5</v>
       </c>
       <c r="H4" t="n">
-        <v>19400</v>
+        <v>20000</v>
       </c>
       <c r="I4" t="n">
         <v>35000</v>
       </c>
       <c r="J4" t="n">
-        <v>0.7522533410608025</v>
+        <v>0.7156638795194469</v>
       </c>
       <c r="K4" t="n">
-        <v>1600</v>
+        <v>1680.75</v>
       </c>
       <c r="L4" t="n">
         <v>35000</v>
@@ -1695,863 +1351,943 @@
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>698</v>
+        <v>689</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>int_rate</t>
+          <t>term</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>9524</v>
       </c>
       <c r="C5" t="n">
-        <v>14.27785174296514</v>
+        <v>41.682486350273</v>
       </c>
       <c r="D5" t="n">
-        <v>4.430159105181627</v>
+        <v>10.20293837881134</v>
       </c>
       <c r="E5" t="n">
-        <v>6.03</v>
+        <v>36</v>
       </c>
       <c r="F5" t="n">
-        <v>11.14</v>
+        <v>36</v>
       </c>
       <c r="G5" t="n">
-        <v>14.09</v>
+        <v>36</v>
       </c>
       <c r="H5" t="n">
-        <v>17.27</v>
+        <v>36</v>
       </c>
       <c r="I5" t="n">
-        <v>26.06</v>
+        <v>60</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2477270312103083</v>
+        <v>1.238631528508025</v>
       </c>
       <c r="K5" t="n">
-        <v>6.03</v>
+        <v>36</v>
       </c>
       <c r="L5" t="n">
-        <v>24.5</v>
+        <v>60</v>
       </c>
       <c r="M5" t="n">
         <v>1</v>
       </c>
       <c r="N5" t="n">
-        <v>0.9524</v>
+        <v>1</v>
       </c>
       <c r="O5" t="n">
         <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>134</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>installment</t>
+          <t>int_rate</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>9524</v>
       </c>
       <c r="C6" t="n">
-        <v>442.6266054178917</v>
+        <v>14.27785174296514</v>
       </c>
       <c r="D6" t="n">
-        <v>244.5221162473253</v>
+        <v>4.430159105181627</v>
       </c>
       <c r="E6" t="n">
-        <v>30.44</v>
+        <v>6.03</v>
       </c>
       <c r="F6" t="n">
-        <v>266.575</v>
+        <v>11.14</v>
       </c>
       <c r="G6" t="n">
-        <v>398.51</v>
+        <v>14.09</v>
       </c>
       <c r="H6" t="n">
-        <v>576.7375000000001</v>
+        <v>17.27</v>
       </c>
       <c r="I6" t="n">
-        <v>1388.45</v>
+        <v>26.06</v>
       </c>
       <c r="J6" t="n">
-        <v>0.9320047875434381</v>
+        <v>0.2477270312103084</v>
       </c>
       <c r="K6" t="n">
-        <v>58.9683</v>
+        <v>6.03</v>
       </c>
       <c r="L6" t="n">
-        <v>1213.7354</v>
+        <v>24.5</v>
       </c>
       <c r="M6" t="n">
         <v>1</v>
       </c>
       <c r="N6" t="n">
-        <v>0.9524</v>
+        <v>1</v>
       </c>
       <c r="O6" t="n">
         <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>5174</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>annual_inc</t>
+          <t>installment</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>9524</v>
       </c>
       <c r="C7" t="n">
-        <v>71655.7522448551</v>
+        <v>442.6266054178917</v>
       </c>
       <c r="D7" t="n">
-        <v>45362.83449458588</v>
+        <v>244.5221162473253</v>
       </c>
       <c r="E7" t="n">
-        <v>7500</v>
+        <v>30.44</v>
       </c>
       <c r="F7" t="n">
-        <v>45000</v>
+        <v>266.575</v>
       </c>
       <c r="G7" t="n">
-        <v>61000</v>
+        <v>398.51</v>
       </c>
       <c r="H7" t="n">
-        <v>86000</v>
+        <v>576.7375000000001</v>
       </c>
       <c r="I7" t="n">
-        <v>1000000</v>
+        <v>1388.45</v>
       </c>
       <c r="J7" t="n">
-        <v>5.006879478282269</v>
+        <v>0.9320047875434381</v>
       </c>
       <c r="K7" t="n">
-        <v>19500</v>
+        <v>58.9683</v>
       </c>
       <c r="L7" t="n">
-        <v>225000</v>
+        <v>1213.7354</v>
       </c>
       <c r="M7" t="n">
         <v>1</v>
       </c>
       <c r="N7" t="n">
-        <v>0.9524</v>
+        <v>1</v>
       </c>
       <c r="O7" t="n">
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>1492</v>
+        <v>5174</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>dti</t>
+          <t>emp_length</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>9524</v>
+        <v>9119</v>
       </c>
       <c r="C8" t="n">
-        <v>17.14692671146577</v>
+        <v>6.088990020835618</v>
       </c>
       <c r="D8" t="n">
-        <v>7.591600903536246</v>
+        <v>3.501151920835093</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F8" t="n">
-        <v>11.52</v>
+        <v>3</v>
       </c>
       <c r="G8" t="n">
-        <v>16.84</v>
+        <v>6</v>
       </c>
       <c r="H8" t="n">
-        <v>22.59</v>
+        <v>10</v>
       </c>
       <c r="I8" t="n">
-        <v>34.98</v>
+        <v>10</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1319907912889219</v>
+        <v>-0.2104844489790758</v>
       </c>
       <c r="K8" t="n">
-        <v>1.9623</v>
+        <v>0.5</v>
       </c>
       <c r="L8" t="n">
-        <v>33.72</v>
+        <v>10</v>
       </c>
       <c r="M8" t="n">
-        <v>0.9996</v>
+        <v>1</v>
       </c>
       <c r="N8" t="n">
-        <v>0.952</v>
+        <v>0.9574758504829903</v>
       </c>
       <c r="O8" t="n">
         <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>2955</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>delinq_2yrs</t>
+          <t>annual_inc</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>9524</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2387652246955061</v>
+        <v>71655.7522448551</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6914554697926136</v>
+        <v>45362.83449458588</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>7500</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>45000</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>61000</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>86000</v>
       </c>
       <c r="I9" t="n">
-        <v>11</v>
+        <v>1000000</v>
       </c>
       <c r="J9" t="n">
-        <v>4.944461797439068</v>
+        <v>5.006879478282269</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>19500</v>
       </c>
       <c r="L9" t="n">
-        <v>3</v>
+        <v>225000</v>
       </c>
       <c r="M9" t="n">
-        <v>0.1975</v>
+        <v>1</v>
       </c>
       <c r="N9" t="n">
-        <v>0.1499</v>
+        <v>1</v>
       </c>
       <c r="O9" t="n">
         <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>11</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>mths_since_last_delinq</t>
+          <t>dti</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4100</v>
+        <v>9524</v>
       </c>
       <c r="C10" t="n">
-        <v>34.98853658536586</v>
+        <v>17.14692671146577</v>
       </c>
       <c r="D10" t="n">
-        <v>21.47450908470911</v>
+        <v>7.591600903536246</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>17</v>
+        <v>11.52</v>
       </c>
       <c r="G10" t="n">
-        <v>32</v>
+        <v>16.84</v>
       </c>
       <c r="H10" t="n">
-        <v>49</v>
+        <v>22.59</v>
       </c>
       <c r="I10" t="n">
-        <v>122</v>
+        <v>34.98</v>
       </c>
       <c r="J10" t="n">
-        <v>0.4635379031754838</v>
+        <v>0.1319907912889234</v>
       </c>
       <c r="K10" t="n">
-        <v>2</v>
+        <v>1.9623</v>
       </c>
       <c r="L10" t="n">
-        <v>81</v>
+        <v>33.72</v>
       </c>
       <c r="M10" t="n">
-        <v>0.9995000000000001</v>
+        <v>0.999580008399832</v>
       </c>
       <c r="N10" t="n">
-        <v>0.4095</v>
+        <v>0.999580008399832</v>
       </c>
       <c r="O10" t="n">
         <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>87</v>
+        <v>2955</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>open_acc</t>
+          <t>delinq_2yrs</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>9524</v>
       </c>
       <c r="C11" t="n">
-        <v>11.04378412431751</v>
+        <v>0.2387652246955061</v>
       </c>
       <c r="D11" t="n">
-        <v>4.56102797240828</v>
+        <v>0.6914554697926136</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="J11" t="n">
-        <v>0.935223057713899</v>
+        <v>4.94446179743907</v>
       </c>
       <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
         <v>3</v>
       </c>
-      <c r="L11" t="n">
-        <v>25</v>
-      </c>
       <c r="M11" t="n">
-        <v>1</v>
+        <v>0.1573918521629567</v>
       </c>
       <c r="N11" t="n">
-        <v>0.9524</v>
+        <v>0.1573918521629567</v>
       </c>
       <c r="O11" t="n">
         <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>36</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>revol_bal</t>
+          <t>mths_since_last_delinq</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>9524</v>
+        <v>4100</v>
       </c>
       <c r="C12" t="n">
-        <v>15982.9982150357</v>
+        <v>34.98853658536586</v>
       </c>
       <c r="D12" t="n">
-        <v>15177.64810529229</v>
+        <v>21.47450908470911</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>7151</v>
+        <v>17</v>
       </c>
       <c r="G12" t="n">
-        <v>12495</v>
+        <v>32</v>
       </c>
       <c r="H12" t="n">
-        <v>20596</v>
+        <v>49</v>
       </c>
       <c r="I12" t="n">
-        <v>376679</v>
+        <v>122</v>
       </c>
       <c r="J12" t="n">
-        <v>5.608316160509967</v>
+        <v>0.4635379031754837</v>
       </c>
       <c r="K12" t="n">
-        <v>412.92</v>
+        <v>2</v>
       </c>
       <c r="L12" t="n">
-        <v>68804.16000000018</v>
+        <v>81</v>
       </c>
       <c r="M12" t="n">
-        <v>0.9975000000000001</v>
+        <v>0.99947501049979</v>
       </c>
       <c r="N12" t="n">
-        <v>0.9499</v>
+        <v>0.4299664006719865</v>
       </c>
       <c r="O12" t="n">
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>8180</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>total_acc</t>
+          <t>open_acc</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>9524</v>
       </c>
       <c r="C13" t="n">
-        <v>24.51763964720706</v>
+        <v>11.04378412431751</v>
       </c>
       <c r="D13" t="n">
-        <v>10.88769258814117</v>
+        <v>4.56102797240828</v>
       </c>
       <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>8</v>
+      </c>
+      <c r="G13" t="n">
+        <v>10</v>
+      </c>
+      <c r="H13" t="n">
+        <v>14</v>
+      </c>
+      <c r="I13" t="n">
+        <v>39</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.9352230577138988</v>
+      </c>
+      <c r="K13" t="n">
         <v>3</v>
       </c>
-      <c r="F13" t="n">
-        <v>17</v>
-      </c>
-      <c r="G13" t="n">
-        <v>23</v>
-      </c>
-      <c r="H13" t="n">
-        <v>31</v>
-      </c>
-      <c r="I13" t="n">
-        <v>68</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0.7221528984225445</v>
-      </c>
-      <c r="K13" t="n">
-        <v>6</v>
-      </c>
       <c r="L13" t="n">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="M13" t="n">
         <v>1</v>
       </c>
       <c r="N13" t="n">
-        <v>0.9524</v>
+        <v>1</v>
       </c>
       <c r="O13" t="n">
         <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>64</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>out_prncp</t>
+          <t>revol_bal</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>9524</v>
       </c>
       <c r="C14" t="n">
-        <v>10253.67422931541</v>
+        <v>15982.9982150357</v>
       </c>
       <c r="D14" t="n">
-        <v>7963.300049631496</v>
+        <v>15177.64810529229</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>4273.3875</v>
+        <v>7151</v>
       </c>
       <c r="G14" t="n">
-        <v>8745.424999999999</v>
+        <v>12495</v>
       </c>
       <c r="H14" t="n">
-        <v>15055.4375</v>
+        <v>20596</v>
       </c>
       <c r="I14" t="n">
-        <v>34413.52</v>
+        <v>376679</v>
       </c>
       <c r="J14" t="n">
-        <v>0.7859300330164416</v>
+        <v>5.608316160509967</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>412.92</v>
       </c>
       <c r="L14" t="n">
-        <v>32680.21800000001</v>
+        <v>68804.16000000018</v>
       </c>
       <c r="M14" t="n">
-        <v>0.8831</v>
+        <v>0.99737505249895</v>
       </c>
       <c r="N14" t="n">
-        <v>0.8355</v>
+        <v>0.99737505249895</v>
       </c>
       <c r="O14" t="n">
         <v>0</v>
       </c>
       <c r="P14" t="n">
-        <v>8224</v>
+        <v>8180</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>total_pymnt</t>
+          <t>total_acc</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>9524</v>
       </c>
       <c r="C15" t="n">
-        <v>5225.24094553339</v>
+        <v>24.51763964720706</v>
       </c>
       <c r="D15" t="n">
-        <v>5499.478657014814</v>
+        <v>10.88769258814117</v>
       </c>
       <c r="E15" t="n">
-        <v>34.14</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
-        <v>1676.3125</v>
+        <v>17</v>
       </c>
       <c r="G15" t="n">
-        <v>3500.04</v>
+        <v>23</v>
       </c>
       <c r="H15" t="n">
-        <v>6736.965</v>
+        <v>31</v>
       </c>
       <c r="I15" t="n">
-        <v>44231.08</v>
+        <v>68</v>
       </c>
       <c r="J15" t="n">
-        <v>2.552874967523885</v>
+        <v>0.7221528984225445</v>
       </c>
       <c r="K15" t="n">
-        <v>260.4607</v>
+        <v>6</v>
       </c>
       <c r="L15" t="n">
-        <v>27150.93400000005</v>
+        <v>56</v>
       </c>
       <c r="M15" t="n">
         <v>1</v>
       </c>
       <c r="N15" t="n">
-        <v>0.9524</v>
+        <v>1</v>
       </c>
       <c r="O15" t="n">
         <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>9282</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>total_rec_prncp</t>
+          <t>out_prncp</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>9524</v>
       </c>
       <c r="C16" t="n">
-        <v>3808.501311423771</v>
+        <v>10253.67422931541</v>
       </c>
       <c r="D16" t="n">
-        <v>4801.501190986038</v>
+        <v>7963.300049631496</v>
       </c>
       <c r="E16" t="n">
-        <v>22.5</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>1027.525</v>
+        <v>4273.3875</v>
       </c>
       <c r="G16" t="n">
-        <v>2237.87</v>
+        <v>8745.424999999999</v>
       </c>
       <c r="H16" t="n">
-        <v>4544.47</v>
+        <v>15055.4375</v>
       </c>
       <c r="I16" t="n">
-        <v>35000.01</v>
+        <v>34413.52</v>
       </c>
       <c r="J16" t="n">
-        <v>3.071417938640482</v>
+        <v>0.7859300330164416</v>
       </c>
       <c r="K16" t="n">
-        <v>143.4852</v>
+        <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>25000</v>
+        <v>32680.21800000001</v>
       </c>
       <c r="M16" t="n">
-        <v>1</v>
+        <v>0.877257454850903</v>
       </c>
       <c r="N16" t="n">
-        <v>0.9524</v>
+        <v>0.877257454850903</v>
       </c>
       <c r="O16" t="n">
         <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>8644</v>
+        <v>8224</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>total_rec_int</t>
+          <t>total_pymnt</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>9524</v>
       </c>
       <c r="C17" t="n">
-        <v>1412.893986770265</v>
+        <v>5225.240945533389</v>
       </c>
       <c r="D17" t="n">
-        <v>1489.22751636475</v>
+        <v>5499.478657014814</v>
       </c>
       <c r="E17" t="n">
-        <v>11.64</v>
+        <v>34.14</v>
       </c>
       <c r="F17" t="n">
-        <v>468.1125</v>
+        <v>1676.3125</v>
       </c>
       <c r="G17" t="n">
-        <v>947</v>
+        <v>3500.04</v>
       </c>
       <c r="H17" t="n">
-        <v>1777.87</v>
+        <v>6736.965</v>
       </c>
       <c r="I17" t="n">
-        <v>13514.55</v>
+        <v>44231.08</v>
       </c>
       <c r="J17" t="n">
-        <v>2.596306533056652</v>
+        <v>2.552874967523885</v>
       </c>
       <c r="K17" t="n">
-        <v>65.79040000000001</v>
+        <v>260.4607</v>
       </c>
       <c r="L17" t="n">
-        <v>7245.8464</v>
+        <v>27150.93400000005</v>
       </c>
       <c r="M17" t="n">
         <v>1</v>
       </c>
       <c r="N17" t="n">
-        <v>0.9524</v>
+        <v>1</v>
       </c>
       <c r="O17" t="n">
         <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>9229</v>
+        <v>9282</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>wtd_loans</t>
+          <t>total_rec_prncp</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
+        <v>9524</v>
+      </c>
+      <c r="C18" t="n">
+        <v>3808.501311423771</v>
+      </c>
+      <c r="D18" t="n">
+        <v>4801.501190986038</v>
+      </c>
+      <c r="E18" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1027.525</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2237.87</v>
+      </c>
+      <c r="H18" t="n">
+        <v>4544.47</v>
+      </c>
+      <c r="I18" t="n">
+        <v>35000.01</v>
+      </c>
+      <c r="J18" t="n">
+        <v>3.071417938640482</v>
+      </c>
+      <c r="K18" t="n">
+        <v>143.4852</v>
+      </c>
+      <c r="L18" t="n">
+        <v>25000</v>
+      </c>
       <c r="M18" t="n">
         <v>1</v>
       </c>
       <c r="N18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O18" t="n">
         <v>0</v>
       </c>
       <c r="P18" t="n">
-        <v>0</v>
+        <v>8644</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>interest_rate</t>
+          <t>total_rec_int</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
+        <v>9524</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1412.893986770265</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1489.22751636475</v>
+      </c>
+      <c r="E19" t="n">
+        <v>11.64</v>
+      </c>
+      <c r="F19" t="n">
+        <v>468.1125</v>
+      </c>
+      <c r="G19" t="n">
+        <v>947</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1777.87</v>
+      </c>
+      <c r="I19" t="n">
+        <v>13514.55</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2.596306533056652</v>
+      </c>
+      <c r="K19" t="n">
+        <v>65.79040000000001</v>
+      </c>
+      <c r="L19" t="n">
+        <v>7245.8464</v>
+      </c>
       <c r="M19" t="n">
         <v>1</v>
       </c>
       <c r="N19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19" t="n">
         <v>0</v>
       </c>
       <c r="P19" t="n">
-        <v>0</v>
+        <v>9229</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>num_rate</t>
+          <t>days_since_earliest_cr_line</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
+        <v>9524</v>
+      </c>
+      <c r="C20" t="n">
+        <v>9485.557328853423</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2891.225051787537</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-16815</v>
+      </c>
+      <c r="F20" t="n">
+        <v>7808.75</v>
+      </c>
+      <c r="G20" t="n">
+        <v>9065</v>
+      </c>
+      <c r="H20" t="n">
+        <v>10856.25</v>
+      </c>
+      <c r="I20" t="n">
+        <v>19694</v>
+      </c>
+      <c r="J20" t="n">
+        <v>-1.374523375552301</v>
+      </c>
+      <c r="K20" t="n">
+        <v>5394.84</v>
+      </c>
+      <c r="L20" t="n">
+        <v>17167.13000000003</v>
+      </c>
       <c r="M20" t="n">
         <v>1</v>
       </c>
       <c r="N20" t="n">
-        <v>0</v>
+        <v>0.99685006299874</v>
       </c>
       <c r="O20" t="n">
-        <v>0</v>
+        <v>0.003149937001259975</v>
       </c>
       <c r="P20" t="n">
-        <v>0</v>
+        <v>5708</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>numrate</t>
+          <t>is_bad_loan</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
+        <v>9524</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.04231415371692566</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.2013154774447118</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" t="n">
+        <v>4.547906444020452</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1</v>
+      </c>
       <c r="M21" t="n">
-        <v>1</v>
+        <v>0.04231415371692566</v>
       </c>
       <c r="N21" t="n">
-        <v>0</v>
+        <v>0.04231415371692566</v>
       </c>
       <c r="O21" t="n">
         <v>0</v>
       </c>
       <c r="P21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>int_rate3</t>
+          <t>is_loan_complete</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>9524</v>
       </c>
       <c r="C22" t="n">
-        <v>14.27785174296514</v>
+        <v>0.124422511549769</v>
       </c>
       <c r="D22" t="n">
-        <v>4.430159105181627</v>
+        <v>0.3300802781212024</v>
       </c>
       <c r="E22" t="n">
-        <v>6.03</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>11.14</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>14.09</v>
+        <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>17.27</v>
+        <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>26.06</v>
+        <v>1</v>
       </c>
       <c r="J22" t="n">
-        <v>0.2477270312103083</v>
+        <v>2.276151588634189</v>
       </c>
       <c r="K22" t="n">
-        <v>6.03</v>
+        <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>24.5</v>
+        <v>1</v>
       </c>
       <c r="M22" t="n">
-        <v>1</v>
+        <v>0.124422511549769</v>
       </c>
       <c r="N22" t="n">
-        <v>0.9524</v>
+        <v>0.124422511549769</v>
       </c>
       <c r="O22" t="n">
         <v>0</v>
       </c>
       <c r="P22" t="n">
-        <v>134</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2591,92 +2327,92 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>term</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>int_rate</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>installment</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>emp_length</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>annual_inc</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>dti</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>delinq_2yrs</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>mths_since_last_delinq</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>open_acc</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>revol_bal</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>total_acc</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>out_prncp</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>total_pymnt</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>total_rec_prncp</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>total_rec_int</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>wtd_loans</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>interest_rate</t>
-        </is>
-      </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>num_rate</t>
+          <t>days_since_earliest_cr_line</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>numrate</t>
+          <t>is_bad_loan</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>int_rate3</t>
+          <t>is_loan_complete</t>
         </is>
       </c>
     </row>
@@ -2690,56 +2426,64 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.002758658134230677</v>
+        <v>0.03840419176342529</v>
       </c>
       <c r="D2" t="n">
-        <v>0.003107879872501092</v>
+        <v>0.0387611569000612</v>
       </c>
       <c r="E2" t="n">
+        <v>0.07909960155307198</v>
+      </c>
+      <c r="F2" t="n">
         <v>0.08405464812229682</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0.02677887360017952</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
+        <v>0.05180279790778151</v>
+      </c>
+      <c r="I2" t="n">
         <v>0.03802762577251442</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>0.01665291442253831</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>0.05519570169120708</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
         <v>-0.0399334907927763</v>
       </c>
-      <c r="K2" t="n">
+      <c r="M2" t="n">
         <v>0.0527291608664317</v>
       </c>
-      <c r="L2" t="n">
+      <c r="N2" t="n">
         <v>0.0152131535348174</v>
       </c>
-      <c r="M2" t="n">
+      <c r="O2" t="n">
         <v>0.06588542302187546</v>
       </c>
-      <c r="N2" t="n">
+      <c r="P2" t="n">
         <v>0.3380550076833274</v>
       </c>
-      <c r="O2" t="n">
+      <c r="Q2" t="n">
         <v>-0.5024187554940663</v>
       </c>
-      <c r="P2" t="n">
+      <c r="R2" t="n">
         <v>-0.4406301697957097</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="S2" t="n">
         <v>-0.4316034520042666</v>
       </c>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
+      <c r="T2" t="n">
+        <v>0.006980658568117399</v>
+      </c>
+      <c r="U2" t="n">
+        <v>-0.1603113661319432</v>
+      </c>
       <c r="V2" t="n">
-        <v>0.08405464812229682</v>
+        <v>-0.2744042973374832</v>
       </c>
     </row>
     <row r="3">
@@ -2749,59 +2493,67 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.002758658134230677</v>
+        <v>0.03840419176342529</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9998900444437675</v>
+        <v>0.999886098386032</v>
       </c>
       <c r="E3" t="n">
+        <v>0.4402810733868834</v>
+      </c>
+      <c r="F3" t="n">
         <v>0.1941498279875427</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>0.9562835370848278</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
+        <v>0.1198135127861392</v>
+      </c>
+      <c r="I3" t="n">
         <v>0.4205685628017545</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>0.03545828149296679</v>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>0.0282814533990339</v>
       </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
         <v>-0.0589214688300067</v>
       </c>
-      <c r="K3" t="n">
+      <c r="M3" t="n">
         <v>0.1892883028886232</v>
       </c>
-      <c r="L3" t="n">
+      <c r="N3" t="n">
         <v>0.3888660111495951</v>
       </c>
-      <c r="M3" t="n">
+      <c r="O3" t="n">
         <v>0.2363881531006886</v>
       </c>
-      <c r="N3" t="n">
+      <c r="P3" t="n">
         <v>0.7977809299311331</v>
       </c>
-      <c r="O3" t="n">
+      <c r="Q3" t="n">
         <v>0.4749048076980654</v>
       </c>
-      <c r="P3" t="n">
+      <c r="R3" t="n">
         <v>0.3498476102998798</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="S3" t="n">
         <v>0.6251592498028142</v>
       </c>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
+      <c r="T3" t="n">
+        <v>0.1661171206430378</v>
+      </c>
+      <c r="U3" t="n">
+        <v>-0.0001829304844254737</v>
+      </c>
       <c r="V3" t="n">
-        <v>0.1941498279875427</v>
+        <v>-0.04441511088009923</v>
       </c>
     </row>
     <row r="4">
@@ -2811,1037 +2563,1325 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.003107879872501092</v>
+        <v>0.0387611569000612</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9998900444437675</v>
+        <v>0.999886098386032</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
+        <v>0.4401089353833854</v>
+      </c>
+      <c r="F4" t="n">
         <v>0.1941217296868053</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>0.9564183935190413</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
+        <v>0.1198359348859457</v>
+      </c>
+      <c r="I4" t="n">
         <v>0.4203611505005494</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>0.03545015295409164</v>
       </c>
-      <c r="I4" t="n">
+      <c r="K4" t="n">
         <v>0.02810348837012933</v>
       </c>
-      <c r="J4" t="n">
+      <c r="L4" t="n">
         <v>-0.05877226517602122</v>
       </c>
-      <c r="K4" t="n">
+      <c r="M4" t="n">
         <v>0.1892757560548846</v>
       </c>
-      <c r="L4" t="n">
+      <c r="N4" t="n">
         <v>0.3887759283679418</v>
       </c>
-      <c r="M4" t="n">
+      <c r="O4" t="n">
         <v>0.2363852694946592</v>
       </c>
-      <c r="N4" t="n">
+      <c r="P4" t="n">
         <v>0.7980634476495118</v>
       </c>
-      <c r="O4" t="n">
+      <c r="Q4" t="n">
         <v>0.4748411203230155</v>
       </c>
-      <c r="P4" t="n">
+      <c r="R4" t="n">
         <v>0.3498126244556855</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="S4" t="n">
         <v>0.6250361005460345</v>
       </c>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
+      <c r="T4" t="n">
+        <v>0.1661181442359846</v>
+      </c>
+      <c r="U4" t="n">
+        <v>-0.0006411910079999735</v>
+      </c>
       <c r="V4" t="n">
-        <v>0.1941217296868053</v>
+        <v>-0.0446331993138875</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>int_rate</t>
+          <t>term</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.08405464812229682</v>
+        <v>0.07909960155307198</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1941498279875427</v>
+        <v>0.4402810733868834</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1941217296868053</v>
+        <v>0.4401089353833854</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1731671862589893</v>
+        <v>0.4689368822728937</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.01748782801329928</v>
+        <v>0.2019219337732875</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1398694758891641</v>
+        <v>0.0820922001157619</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1212891637330143</v>
+        <v>0.08467803980741462</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.07852659604476984</v>
+        <v>0.0749469379226963</v>
       </c>
       <c r="K5" t="n">
-        <v>0.00986005203253576</v>
+        <v>0.0227142645566989</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.004952812616559396</v>
+        <v>-0.03263237094229556</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.01718064079404476</v>
+        <v>0.06808899207187843</v>
       </c>
       <c r="N5" t="n">
-        <v>0.204750449091043</v>
+        <v>0.1238044353517985</v>
       </c>
       <c r="O5" t="n">
-        <v>0.07615432067946877</v>
+        <v>0.1130882120797538</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.04136073442324357</v>
+        <v>0.4481072723141252</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.4134771318529046</v>
-      </c>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr"/>
+        <v>0.104759833219231</v>
+      </c>
+      <c r="R5" t="n">
+        <v>-0.01143978202249202</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.4236514226390913</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.06218454464483823</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.03261488676066457</v>
+      </c>
       <c r="V5" t="n">
-        <v>1</v>
+        <v>-0.03260676567439146</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>installment</t>
+          <t>int_rate</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.02677887360017952</v>
+        <v>0.08405464812229682</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9562835370848278</v>
+        <v>0.1941498279875427</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9564183935190413</v>
+        <v>0.1941217296868053</v>
       </c>
       <c r="E6" t="n">
+        <v>0.4689368822728937</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
         <v>0.1731671862589893</v>
       </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.423917962199917</v>
-      </c>
       <c r="H6" t="n">
-        <v>0.03073044662711546</v>
+        <v>0.02386559237228218</v>
       </c>
       <c r="I6" t="n">
-        <v>0.03801547398382302</v>
+        <v>-0.01748782801329928</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.05789857950686371</v>
+        <v>0.1398694758891641</v>
       </c>
       <c r="K6" t="n">
-        <v>0.1857994463410156</v>
+        <v>0.1212891637330143</v>
       </c>
       <c r="L6" t="n">
-        <v>0.3771697811069278</v>
+        <v>-0.07852659604476984</v>
       </c>
       <c r="M6" t="n">
-        <v>0.2186546603594354</v>
+        <v>0.00986005203253576</v>
       </c>
       <c r="N6" t="n">
-        <v>0.7330585106641035</v>
+        <v>-0.004952812616559396</v>
       </c>
       <c r="O6" t="n">
-        <v>0.4915280215745405</v>
+        <v>-0.01718064079404476</v>
       </c>
       <c r="P6" t="n">
-        <v>0.3817157724703686</v>
+        <v>0.204750449091043</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.5835634632017765</v>
-      </c>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
+        <v>0.07615432067946877</v>
+      </c>
+      <c r="R6" t="n">
+        <v>-0.04136073442324357</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.4134771318529046</v>
+      </c>
+      <c r="T6" t="n">
+        <v>-0.07510267566959614</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.08518786119915019</v>
+      </c>
       <c r="V6" t="n">
-        <v>0.1731671862589893</v>
+        <v>-0.008213264762011001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>annual_inc</t>
+          <t>installment</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.03802762577251442</v>
+        <v>0.02677887360017952</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4205685628017545</v>
+        <v>0.9562835370848278</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4203611505005494</v>
+        <v>0.9564183935190413</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.01748782801329928</v>
+        <v>0.2019219337732875</v>
       </c>
       <c r="F7" t="n">
+        <v>0.1731671862589893</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.1070019900562518</v>
+      </c>
+      <c r="I7" t="n">
         <v>0.423917962199917</v>
       </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-0.2324297468434838</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.08688911866216703</v>
-      </c>
       <c r="J7" t="n">
-        <v>-0.07856226839342052</v>
+        <v>0.03073044662711546</v>
       </c>
       <c r="K7" t="n">
-        <v>0.1768466527324548</v>
+        <v>0.03801547398382302</v>
       </c>
       <c r="L7" t="n">
-        <v>0.3882204517574174</v>
+        <v>-0.05789857950686371</v>
       </c>
       <c r="M7" t="n">
-        <v>0.254963332431854</v>
+        <v>0.1857994463410156</v>
       </c>
       <c r="N7" t="n">
-        <v>0.3206019063834847</v>
+        <v>0.3771697811069278</v>
       </c>
       <c r="O7" t="n">
-        <v>0.219034318428889</v>
+        <v>0.2186546603594354</v>
       </c>
       <c r="P7" t="n">
-        <v>0.18835592828002</v>
+        <v>0.7330585106641035</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.2021922516848149</v>
-      </c>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
+        <v>0.4915280215745405</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.3817157724703686</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.5835634632017765</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.1514680764850076</v>
+      </c>
+      <c r="U7" t="n">
+        <v>-0.001182435165376681</v>
+      </c>
       <c r="V7" t="n">
-        <v>-0.01748782801329928</v>
+        <v>-0.03694285708325936</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>dti</t>
+          <t>emp_length</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.01665291442253831</v>
+        <v>0.05180279790778151</v>
       </c>
       <c r="C8" t="n">
-        <v>0.03545828149296679</v>
+        <v>0.1198135127861392</v>
       </c>
       <c r="D8" t="n">
-        <v>0.03545015295409164</v>
+        <v>0.1198359348859457</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1398694758891641</v>
+        <v>0.0820922001157619</v>
       </c>
       <c r="F8" t="n">
-        <v>0.03073044662711546</v>
+        <v>0.02386559237228218</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.2324297468434838</v>
+        <v>0.1070019900562518</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.01893612702399092</v>
+        <v>0.07450770647371426</v>
       </c>
       <c r="J8" t="n">
-        <v>0.05840874172961694</v>
+        <v>0.04753710944963281</v>
       </c>
       <c r="K8" t="n">
-        <v>0.2836445299317972</v>
+        <v>0.05187526133162706</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1571396891428203</v>
+        <v>-0.04097852575421496</v>
       </c>
       <c r="M8" t="n">
-        <v>0.223144958723226</v>
+        <v>0.04422422858336939</v>
       </c>
       <c r="N8" t="n">
-        <v>0.07371813408206847</v>
+        <v>0.1204446507723376</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.04647675960277939</v>
+        <v>0.1230107212292848</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.07205290126199961</v>
+        <v>0.1140433167818606</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.06011735000677031</v>
-      </c>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
+        <v>0.02654305557925321</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.01219696967673465</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.05907927554057753</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.208291418172327</v>
+      </c>
+      <c r="U8" t="n">
+        <v>-0.01195888095377732</v>
+      </c>
       <c r="V8" t="n">
-        <v>0.1398694758891642</v>
+        <v>-0.01194804894314194</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>delinq_2yrs</t>
+          <t>annual_inc</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.05519570169120708</v>
+        <v>0.03802762577251442</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0282814533990339</v>
+        <v>0.4205685628017545</v>
       </c>
       <c r="D9" t="n">
-        <v>0.02810348837012933</v>
+        <v>0.4203611505005494</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1212891637330143</v>
+        <v>0.08467803980741462</v>
       </c>
       <c r="F9" t="n">
-        <v>0.03801547398382302</v>
+        <v>-0.01748782801329928</v>
       </c>
       <c r="G9" t="n">
+        <v>0.423917962199917</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.07450770647371426</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-0.2324297468434838</v>
+      </c>
+      <c r="K9" t="n">
         <v>0.08688911866216703</v>
       </c>
-      <c r="H9" t="n">
-        <v>-0.01893612702399092</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" t="n">
-        <v>-0.5963494687200263</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.05551983298183635</v>
-      </c>
       <c r="L9" t="n">
-        <v>-0.008651667991617595</v>
+        <v>-0.07856226839342052</v>
       </c>
       <c r="M9" t="n">
-        <v>0.1459271807771905</v>
+        <v>0.1768466527324548</v>
       </c>
       <c r="N9" t="n">
-        <v>0.02764566861249088</v>
+        <v>0.3882204517574174</v>
       </c>
       <c r="O9" t="n">
-        <v>0.0007883074751746857</v>
+        <v>0.254963332431854</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.007085297458639338</v>
+        <v>0.3206019063834847</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.02566563047928291</v>
-      </c>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
+        <v>0.219034318428889</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.18835592828002</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.2021922516848149</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.1696062477772514</v>
+      </c>
+      <c r="U9" t="n">
+        <v>-0.0474272592357885</v>
+      </c>
       <c r="V9" t="n">
-        <v>0.1212891637330143</v>
+        <v>-0.005945600067037826</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>mths_since_last_delinq</t>
+          <t>dti</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.0399334907927763</v>
+        <v>0.01665291442253831</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.0589214688300067</v>
+        <v>0.03545828149296679</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.05877226517602122</v>
+        <v>0.03545015295409164</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.07852659604476984</v>
+        <v>0.0749469379226963</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.05789857950686371</v>
+        <v>0.1398694758891641</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.07856226839342052</v>
+        <v>0.03073044662711546</v>
       </c>
       <c r="H10" t="n">
+        <v>0.04753710944963281</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-0.2324297468434838</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-0.01893612702399092</v>
+      </c>
+      <c r="L10" t="n">
         <v>0.05840874172961694</v>
       </c>
-      <c r="I10" t="n">
-        <v>-0.5963494687200263</v>
-      </c>
-      <c r="J10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" t="n">
-        <v>-0.04389848919105896</v>
-      </c>
-      <c r="L10" t="n">
-        <v>-0.03888349553078527</v>
-      </c>
       <c r="M10" t="n">
-        <v>-0.08641451790865633</v>
+        <v>0.2836445299317972</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.05174030930396432</v>
+        <v>0.1571396891428203</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.01023138657405276</v>
+        <v>0.223144958723226</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.004953199577505767</v>
+        <v>0.07371813408206847</v>
       </c>
       <c r="Q10" t="n">
-        <v>-0.02129202842353808</v>
-      </c>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
+        <v>-0.04647675960277939</v>
+      </c>
+      <c r="R10" t="n">
+        <v>-0.07205290126199961</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.06011735000677031</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.02570551850316669</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0.04767936119107717</v>
+      </c>
       <c r="V10" t="n">
-        <v>-0.07852659604476984</v>
+        <v>-0.04378175800263649</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>open_acc</t>
+          <t>delinq_2yrs</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.0527291608664317</v>
+        <v>0.05519570169120708</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1892883028886232</v>
+        <v>0.0282814533990339</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1892757560548846</v>
+        <v>0.02810348837012933</v>
       </c>
       <c r="E11" t="n">
-        <v>0.00986005203253576</v>
+        <v>0.0227142645566989</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1857994463410156</v>
+        <v>0.1212891637330143</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1768466527324548</v>
+        <v>0.03801547398382302</v>
       </c>
       <c r="H11" t="n">
-        <v>0.2836445299317972</v>
+        <v>0.05187526133162706</v>
       </c>
       <c r="I11" t="n">
+        <v>0.08688911866216703</v>
+      </c>
+      <c r="J11" t="n">
+        <v>-0.01893612702399092</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" t="n">
+        <v>-0.5963494687200263</v>
+      </c>
+      <c r="M11" t="n">
         <v>0.05551983298183635</v>
       </c>
-      <c r="J11" t="n">
-        <v>-0.04389848919105896</v>
-      </c>
-      <c r="K11" t="n">
-        <v>1</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.2459803945734496</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0.6725838570134584</v>
-      </c>
       <c r="N11" t="n">
-        <v>0.1804948334969939</v>
+        <v>-0.008651667991617595</v>
       </c>
       <c r="O11" t="n">
-        <v>0.04314122474517844</v>
+        <v>0.1459271807771905</v>
       </c>
       <c r="P11" t="n">
-        <v>0.02266399463343549</v>
+        <v>0.02764566861249088</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.08624200959699159</v>
-      </c>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
+        <v>0.0007883074751746857</v>
+      </c>
+      <c r="R11" t="n">
+        <v>-0.007085297458639338</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.02566563047928291</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.07902408682487821</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.003604092536699194</v>
+      </c>
       <c r="V11" t="n">
-        <v>0.009860052032535765</v>
+        <v>0.007850604993533204</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>revol_bal</t>
+          <t>mths_since_last_delinq</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.0152131535348174</v>
+        <v>-0.0399334907927763</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3888660111495951</v>
+        <v>-0.0589214688300067</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3887759283679418</v>
+        <v>-0.05877226517602122</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.004952812616559396</v>
+        <v>-0.03263237094229556</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3771697811069278</v>
+        <v>-0.07852659604476984</v>
       </c>
       <c r="G12" t="n">
-        <v>0.3882204517574174</v>
+        <v>-0.05789857950686371</v>
       </c>
       <c r="H12" t="n">
-        <v>0.1571396891428203</v>
+        <v>-0.04097852575421496</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.008651667991617595</v>
+        <v>-0.07856226839342052</v>
       </c>
       <c r="J12" t="n">
+        <v>0.05840874172961694</v>
+      </c>
+      <c r="K12" t="n">
+        <v>-0.5963494687200263</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" t="n">
+        <v>-0.04389848919105896</v>
+      </c>
+      <c r="N12" t="n">
         <v>-0.03888349553078527</v>
       </c>
-      <c r="K12" t="n">
-        <v>0.2459803945734496</v>
-      </c>
-      <c r="L12" t="n">
-        <v>1</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0.2401895363206639</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.3245181180097181</v>
-      </c>
       <c r="O12" t="n">
-        <v>0.1603961446558881</v>
+        <v>-0.08641451790865633</v>
       </c>
       <c r="P12" t="n">
-        <v>0.1228436597662884</v>
+        <v>-0.05174030930396432</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.1965516568599378</v>
-      </c>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
+        <v>-0.01023138657405276</v>
+      </c>
+      <c r="R12" t="n">
+        <v>-0.004953199577505767</v>
+      </c>
+      <c r="S12" t="n">
+        <v>-0.02129202842353808</v>
+      </c>
+      <c r="T12" t="n">
+        <v>-0.0485692572930579</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0.01975795882392319</v>
+      </c>
       <c r="V12" t="n">
-        <v>-0.004952812616559412</v>
+        <v>-0.01871022625356622</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>total_acc</t>
+          <t>open_acc</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.06588542302187546</v>
+        <v>0.0527291608664317</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2363881531006886</v>
+        <v>0.1892883028886232</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2363852694946592</v>
+        <v>0.1892757560548846</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.01718064079404476</v>
+        <v>0.06808899207187843</v>
       </c>
       <c r="F13" t="n">
-        <v>0.2186546603594354</v>
+        <v>0.00986005203253576</v>
       </c>
       <c r="G13" t="n">
-        <v>0.254963332431854</v>
+        <v>0.1857994463410156</v>
       </c>
       <c r="H13" t="n">
-        <v>0.223144958723226</v>
+        <v>0.04422422858336939</v>
       </c>
       <c r="I13" t="n">
-        <v>0.1459271807771905</v>
+        <v>0.1768466527324548</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.08641451790865633</v>
+        <v>0.2836445299317972</v>
       </c>
       <c r="K13" t="n">
+        <v>0.05551983298183635</v>
+      </c>
+      <c r="L13" t="n">
+        <v>-0.04389848919105896</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.2459803945734496</v>
+      </c>
+      <c r="O13" t="n">
         <v>0.6725838570134584</v>
       </c>
-      <c r="L13" t="n">
-        <v>0.2401895363206639</v>
-      </c>
-      <c r="M13" t="n">
-        <v>1</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0.1966763603789857</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0.09194795191689062</v>
-      </c>
       <c r="P13" t="n">
-        <v>0.07360715548002836</v>
+        <v>0.1804948334969939</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.1026869444300147</v>
-      </c>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
+        <v>0.04314122474517844</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.02266399463343549</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.08624200959699159</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.1403058941212592</v>
+      </c>
+      <c r="U13" t="n">
+        <v>-0.02214586290288992</v>
+      </c>
       <c r="V13" t="n">
-        <v>-0.01718064079404476</v>
+        <v>-0.03758714535869852</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>out_prncp</t>
+          <t>revol_bal</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.3380550076833274</v>
+        <v>0.0152131535348174</v>
       </c>
       <c r="C14" t="n">
-        <v>0.7977809299311331</v>
+        <v>0.3888660111495951</v>
       </c>
       <c r="D14" t="n">
-        <v>0.7980634476495118</v>
+        <v>0.3887759283679418</v>
       </c>
       <c r="E14" t="n">
-        <v>0.204750449091043</v>
+        <v>0.1238044353517985</v>
       </c>
       <c r="F14" t="n">
-        <v>0.7330585106641035</v>
+        <v>-0.004952812616559396</v>
       </c>
       <c r="G14" t="n">
-        <v>0.3206019063834847</v>
+        <v>0.3771697811069278</v>
       </c>
       <c r="H14" t="n">
-        <v>0.07371813408206847</v>
+        <v>0.1204446507723376</v>
       </c>
       <c r="I14" t="n">
-        <v>0.02764566861249088</v>
+        <v>0.3882204517574174</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.05174030930396432</v>
+        <v>0.1571396891428203</v>
       </c>
       <c r="K14" t="n">
-        <v>0.1804948334969939</v>
+        <v>-0.008651667991617595</v>
       </c>
       <c r="L14" t="n">
+        <v>-0.03888349553078527</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.2459803945734496</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.2401895363206639</v>
+      </c>
+      <c r="P14" t="n">
         <v>0.3245181180097181</v>
       </c>
-      <c r="M14" t="n">
-        <v>0.1966763603789857</v>
-      </c>
-      <c r="N14" t="n">
-        <v>1</v>
-      </c>
-      <c r="O14" t="n">
-        <v>-0.08963256531058407</v>
-      </c>
-      <c r="P14" t="n">
-        <v>-0.23271280367644</v>
-      </c>
       <c r="Q14" t="n">
-        <v>0.4225122892174757</v>
-      </c>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
+        <v>0.1603961446558881</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.1228436597662884</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.1965516568599378</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.2089714180249067</v>
+      </c>
+      <c r="U14" t="n">
+        <v>-0.02355644545207384</v>
+      </c>
       <c r="V14" t="n">
-        <v>0.2047504490910431</v>
+        <v>-0.03519569572995011</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>total_pymnt</t>
+          <t>total_acc</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.5024187554940663</v>
+        <v>0.06588542302187546</v>
       </c>
       <c r="C15" t="n">
-        <v>0.4749048076980654</v>
+        <v>0.2363881531006886</v>
       </c>
       <c r="D15" t="n">
-        <v>0.4748411203230155</v>
+        <v>0.2363852694946592</v>
       </c>
       <c r="E15" t="n">
-        <v>0.07615432067946877</v>
+        <v>0.1130882120797538</v>
       </c>
       <c r="F15" t="n">
-        <v>0.4915280215745405</v>
+        <v>-0.01718064079404476</v>
       </c>
       <c r="G15" t="n">
-        <v>0.219034318428889</v>
+        <v>0.2186546603594354</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.04647675960277939</v>
+        <v>0.1230107212292848</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0007883074751746857</v>
+        <v>0.254963332431854</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.01023138657405276</v>
+        <v>0.223144958723226</v>
       </c>
       <c r="K15" t="n">
-        <v>0.04314122474517844</v>
+        <v>0.1459271807771905</v>
       </c>
       <c r="L15" t="n">
-        <v>0.1603961446558881</v>
+        <v>-0.08641451790865633</v>
       </c>
       <c r="M15" t="n">
+        <v>0.6725838570134584</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.2401895363206639</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.1966763603789857</v>
+      </c>
+      <c r="Q15" t="n">
         <v>0.09194795191689062</v>
       </c>
-      <c r="N15" t="n">
-        <v>-0.08963256531058407</v>
-      </c>
-      <c r="O15" t="n">
-        <v>1</v>
-      </c>
-      <c r="P15" t="n">
-        <v>0.9671908108771529</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>0.5751723049682733</v>
-      </c>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
+      <c r="R15" t="n">
+        <v>0.07360715548002836</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.1026869444300147</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0.2644585520261899</v>
+      </c>
+      <c r="U15" t="n">
+        <v>-0.0304990156412813</v>
+      </c>
       <c r="V15" t="n">
-        <v>0.07615432067946878</v>
+        <v>0.006913214874031668</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>total_rec_prncp</t>
+          <t>out_prncp</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.4406301697957097</v>
+        <v>0.3380550076833274</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3498476102998798</v>
+        <v>0.7977809299311331</v>
       </c>
       <c r="D16" t="n">
-        <v>0.3498126244556855</v>
+        <v>0.7980634476495118</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.04136073442324357</v>
+        <v>0.4481072723141252</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3817157724703686</v>
+        <v>0.204750449091043</v>
       </c>
       <c r="G16" t="n">
-        <v>0.18835592828002</v>
+        <v>0.7330585106641035</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.07205290126199961</v>
+        <v>0.1140433167818606</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.007085297458639338</v>
+        <v>0.3206019063834847</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.004953199577505767</v>
+        <v>0.07371813408206847</v>
       </c>
       <c r="K16" t="n">
-        <v>0.02266399463343549</v>
+        <v>0.02764566861249088</v>
       </c>
       <c r="L16" t="n">
-        <v>0.1228436597662884</v>
+        <v>-0.05174030930396432</v>
       </c>
       <c r="M16" t="n">
-        <v>0.07360715548002836</v>
+        <v>0.1804948334969939</v>
       </c>
       <c r="N16" t="n">
+        <v>0.3245181180097181</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.1966763603789857</v>
+      </c>
+      <c r="P16" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>-0.08963256531058407</v>
+      </c>
+      <c r="R16" t="n">
         <v>-0.23271280367644</v>
       </c>
-      <c r="O16" t="n">
-        <v>0.9671908108771529</v>
-      </c>
-      <c r="P16" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>0.3486961605958074</v>
-      </c>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr"/>
+      <c r="S16" t="n">
+        <v>0.4225122892174757</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.1304230089706273</v>
+      </c>
+      <c r="U16" t="n">
+        <v>-0.1148139475700935</v>
+      </c>
       <c r="V16" t="n">
-        <v>-0.04136073442324359</v>
+        <v>-0.4760538067900744</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>total_rec_int</t>
+          <t>total_pymnt</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.4316034520042666</v>
+        <v>-0.5024187554940663</v>
       </c>
       <c r="C17" t="n">
-        <v>0.6251592498028142</v>
+        <v>0.4749048076980654</v>
       </c>
       <c r="D17" t="n">
-        <v>0.6250361005460345</v>
+        <v>0.4748411203230155</v>
       </c>
       <c r="E17" t="n">
-        <v>0.4134771318529046</v>
+        <v>0.104759833219231</v>
       </c>
       <c r="F17" t="n">
-        <v>0.5835634632017765</v>
+        <v>0.07615432067946877</v>
       </c>
       <c r="G17" t="n">
-        <v>0.2021922516848149</v>
+        <v>0.4915280215745405</v>
       </c>
       <c r="H17" t="n">
-        <v>0.06011735000677031</v>
+        <v>0.02654305557925321</v>
       </c>
       <c r="I17" t="n">
-        <v>0.02566563047928291</v>
+        <v>0.219034318428889</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.02129202842353808</v>
+        <v>-0.04647675960277939</v>
       </c>
       <c r="K17" t="n">
-        <v>0.08624200959699159</v>
+        <v>0.0007883074751746857</v>
       </c>
       <c r="L17" t="n">
-        <v>0.1965516568599378</v>
+        <v>-0.01023138657405276</v>
       </c>
       <c r="M17" t="n">
-        <v>0.1026869444300147</v>
+        <v>0.04314122474517844</v>
       </c>
       <c r="N17" t="n">
-        <v>0.4225122892174757</v>
+        <v>0.1603961446558881</v>
       </c>
       <c r="O17" t="n">
+        <v>0.09194795191689062</v>
+      </c>
+      <c r="P17" t="n">
+        <v>-0.08963256531058407</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>1</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.9671908108771529</v>
+      </c>
+      <c r="S17" t="n">
         <v>0.5751723049682733</v>
       </c>
-      <c r="P17" t="n">
-        <v>0.3486961605958074</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>1</v>
-      </c>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
-      <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
+      <c r="T17" t="n">
+        <v>0.07571824477505003</v>
+      </c>
+      <c r="U17" t="n">
+        <v>-0.04586977316652776</v>
+      </c>
       <c r="V17" t="n">
-        <v>0.4134771318529046</v>
+        <v>0.4843362776956006</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>wtd_loans</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr"/>
-      <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr"/>
-      <c r="T18" t="inlineStr"/>
-      <c r="U18" t="inlineStr"/>
-      <c r="V18" t="inlineStr"/>
+          <t>total_rec_prncp</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>-0.4406301697957097</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.3498476102998798</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.3498126244556855</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-0.01143978202249202</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-0.04136073442324357</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.3817157724703686</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.01219696967673465</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.18835592828002</v>
+      </c>
+      <c r="J18" t="n">
+        <v>-0.07205290126199961</v>
+      </c>
+      <c r="K18" t="n">
+        <v>-0.007085297458639338</v>
+      </c>
+      <c r="L18" t="n">
+        <v>-0.004953199577505767</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.02266399463343549</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.1228436597662884</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.07360715548002836</v>
+      </c>
+      <c r="P18" t="n">
+        <v>-0.23271280367644</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.9671908108771529</v>
+      </c>
+      <c r="R18" t="n">
+        <v>1</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.3486961605958074</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.06615566138824079</v>
+      </c>
+      <c r="U18" t="n">
+        <v>-0.06582713542357647</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0.5713800206231137</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>interest_rate</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="inlineStr"/>
-      <c r="S19" t="inlineStr"/>
-      <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr"/>
-      <c r="V19" t="inlineStr"/>
+          <t>total_rec_int</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>-0.4316034520042666</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.6251592498028142</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.6250361005460345</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.4236514226390913</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.4134771318529046</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.5835634632017765</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.05907927554057753</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.2021922516848149</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.06011735000677031</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.02566563047928291</v>
+      </c>
+      <c r="L19" t="n">
+        <v>-0.02129202842353808</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.08624200959699159</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.1965516568599378</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.1026869444300147</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.4225122892174757</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.5751723049682733</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.3486961605958074</v>
+      </c>
+      <c r="S19" t="n">
+        <v>1</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0.06695362632316953</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0.03089087474106218</v>
+      </c>
+      <c r="V19" t="n">
+        <v>-0.06023418385599091</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>num_rate</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
-      <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="inlineStr"/>
-      <c r="S20" t="inlineStr"/>
-      <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
-      <c r="V20" t="inlineStr"/>
+          <t>days_since_earliest_cr_line</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.006980658568117399</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.1661171206430378</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.1661181442359846</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.06218454464483823</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-0.07510267566959614</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.1514680764850076</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.208291418172327</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.1696062477772514</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.02570551850316669</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.07902408682487821</v>
+      </c>
+      <c r="L20" t="n">
+        <v>-0.0485692572930579</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.1403058941212592</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.2089714180249067</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.2644585520261899</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.1304230089706273</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.07571824477505003</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.06615566138824079</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.06695362632316953</v>
+      </c>
+      <c r="T20" t="n">
+        <v>1</v>
+      </c>
+      <c r="U20" t="n">
+        <v>-0.01671931638547591</v>
+      </c>
+      <c r="V20" t="n">
+        <v>-0.01578291618820323</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>numrate</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr"/>
-      <c r="T21" t="inlineStr"/>
-      <c r="U21" t="inlineStr"/>
-      <c r="V21" t="inlineStr"/>
+          <t>is_bad_loan</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-0.1603113661319432</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-0.0001829304844254737</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-0.0006411910079999735</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.03261488676066457</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.08518786119915019</v>
+      </c>
+      <c r="G21" t="n">
+        <v>-0.001182435165376681</v>
+      </c>
+      <c r="H21" t="n">
+        <v>-0.01195888095377732</v>
+      </c>
+      <c r="I21" t="n">
+        <v>-0.0474272592357885</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.04767936119107717</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.003604092536699194</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.01975795882392319</v>
+      </c>
+      <c r="M21" t="n">
+        <v>-0.02214586290288992</v>
+      </c>
+      <c r="N21" t="n">
+        <v>-0.02355644545207384</v>
+      </c>
+      <c r="O21" t="n">
+        <v>-0.0304990156412813</v>
+      </c>
+      <c r="P21" t="n">
+        <v>-0.1148139475700935</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>-0.04586977316652776</v>
+      </c>
+      <c r="R21" t="n">
+        <v>-0.06582713542357647</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0.03089087474106218</v>
+      </c>
+      <c r="T21" t="n">
+        <v>-0.01671931638547591</v>
+      </c>
+      <c r="U21" t="n">
+        <v>1</v>
+      </c>
+      <c r="V21" t="n">
+        <v>0.2905436328020715</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>int_rate3</t>
+          <t>is_loan_complete</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.08405464812229682</v>
+        <v>-0.2744042973374832</v>
       </c>
       <c r="C22" t="n">
-        <v>0.1941498279875427</v>
+        <v>-0.04441511088009923</v>
       </c>
       <c r="D22" t="n">
-        <v>0.1941217296868053</v>
+        <v>-0.0446331993138875</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>-0.03260676567439146</v>
       </c>
       <c r="F22" t="n">
-        <v>0.1731671862589893</v>
+        <v>-0.008213264762011001</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.01748782801329928</v>
+        <v>-0.03694285708325936</v>
       </c>
       <c r="H22" t="n">
-        <v>0.1398694758891642</v>
+        <v>-0.01194804894314194</v>
       </c>
       <c r="I22" t="n">
-        <v>0.1212891637330143</v>
+        <v>-0.005945600067037826</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.07852659604476984</v>
+        <v>-0.04378175800263649</v>
       </c>
       <c r="K22" t="n">
-        <v>0.009860052032535765</v>
+        <v>0.007850604993533204</v>
       </c>
       <c r="L22" t="n">
-        <v>-0.004952812616559412</v>
+        <v>-0.01871022625356622</v>
       </c>
       <c r="M22" t="n">
-        <v>-0.01718064079404476</v>
+        <v>-0.03758714535869852</v>
       </c>
       <c r="N22" t="n">
-        <v>0.2047504490910431</v>
+        <v>-0.03519569572995011</v>
       </c>
       <c r="O22" t="n">
-        <v>0.07615432067946878</v>
+        <v>0.006913214874031668</v>
       </c>
       <c r="P22" t="n">
-        <v>-0.04136073442324359</v>
+        <v>-0.4760538067900744</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.4134771318529046</v>
-      </c>
-      <c r="R22" t="inlineStr"/>
-      <c r="S22" t="inlineStr"/>
-      <c r="T22" t="inlineStr"/>
-      <c r="U22" t="inlineStr"/>
+        <v>0.4843362776956006</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0.5713800206231137</v>
+      </c>
+      <c r="S22" t="n">
+        <v>-0.06023418385599091</v>
+      </c>
+      <c r="T22" t="n">
+        <v>-0.01578291618820323</v>
+      </c>
+      <c r="U22" t="n">
+        <v>0.2905436328020715</v>
+      </c>
       <c r="V22" t="n">
         <v>1</v>
       </c>

</xml_diff>